<commit_message>
1. add comparing figures 2. removed temp files
</commit_message>
<xml_diff>
--- a/20_Experiments/false_positive_20180214.xlsx
+++ b/20_Experiments/false_positive_20180214.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\20_박사과정\20_논문\AntiDistributedCrawler_by_NodeReducing_20171120\20_Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/Work/10_Developement/anti-crawler/20_Experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="10005" xr2:uid="{111D200E-12FF-4DF6-AD90-B58E2928114E}"/>
+    <workbookView xWindow="29740" yWindow="-7200" windowWidth="19820" windowHeight="19460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="시트1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$B$2:$G$31</definedName>
+    <definedName name="ltm_frq_comp" localSheetId="2">시트1!$B$2:$F$16</definedName>
+    <definedName name="ltm_frq_comp" localSheetId="1">Sheet1!$B$2:$H$102</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,15 +37,51 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{7BE9AD36-8360-47E7-A81E-929504D44E10}" keepAlive="1" name="쿼리 - day_traffic_fp" description="통합 문서의 'day_traffic_fp' 쿼리에 대한 연결입니다." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="쿼리 - day_traffic_fp" description="통합 문서의 'day_traffic_fp' 쿼리에 대한 연결입니다." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=day_traffic_fp;Extended Properties=&quot;&quot;" command="SELECT * FROM [day_traffic_fp]"/>
+  </connection>
+  <connection id="2" name="ltm_frq_comp" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/user/Documents/Work/10_Developement/anti-crawler/20_Experiments/ltm_frq_comp.csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="ltm_frq_comp1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/user/Documents/Work/10_Developement/anti-crawler/20_Experiments/ltm_frq_comp.csv" comma="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="131">
   <si>
     <t>Column1</t>
   </si>
@@ -405,19 +450,45 @@
   </si>
   <si>
     <t>2175</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>BLOCK_LTM</t>
+  </si>
+  <si>
+    <t>FalsePos_LTM</t>
+  </si>
+  <si>
+    <t>BLOCK_FRQ</t>
+  </si>
+  <si>
+    <t>FalsePos_FRQ</t>
+  </si>
+  <si>
+    <t>LIMIT_LTM</t>
+  </si>
+  <si>
+    <t>LIMIT_FRQ</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="6">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="183" formatCode="0.000000000"/>
-    <numFmt numFmtId="185" formatCode="#,##0_ "/>
-    <numFmt numFmtId="190" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="210" formatCode="0.0000000000_);[Red]\(0.0000000000\)"/>
-    <numFmt numFmtId="213" formatCode="0.0000000000000_);[Red]\(0.0000000000000\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0.000000000"/>
+    <numFmt numFmtId="178" formatCode="#,##0_ "/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="180" formatCode="0.0000000000_);[Red]\(0.0000000000\)"/>
+    <numFmt numFmtId="181" formatCode="0.0000000000000_);[Red]\(0.0000000000000\)"/>
+    <numFmt numFmtId="185" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -453,15 +524,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -471,113 +578,259 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -585,11 +838,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -623,57 +876,192 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="210" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="213" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="쉼표[0]" xfId="1" builtinId="6"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -816,6 +1204,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -830,12 +1234,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -862,7 +1268,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{9C1C43D3-79B8-4F1C-9A49-85EF743BADAC}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="11"/>
       <tableStyleElement type="headerRow" dxfId="10"/>
     </tableStyle>
@@ -879,7 +1285,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{5B4883D1-CAC1-43B7-80C5-1C47BCCCE087}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
     <queryTableFields count="6">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -893,16 +1299,24 @@
 </queryTable>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ltm_frq_comp" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ltm_frq_comp" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AFA0D2A-4F9B-4FB7-822E-E2560B551F06}" name="day_traffic_fp" displayName="day_traffic_fp" ref="B2:G31" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="B2:G31" xr:uid="{8A80AB1C-8D84-416A-BAC1-E163BB2A5A85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="day_traffic_fp" displayName="day_traffic_fp" ref="B2:G31" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B2:G31"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1FFF86BB-754F-4E8B-AB1B-36FA9915A0A7}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{63C20142-CE3B-497C-92BE-D962A95F62B9}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{CF084FFC-DDE2-42BA-AF04-397A4C43608F}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{CF302862-B122-4B7D-8FAC-2C7B9D02625C}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{782CBBF2-1552-4CE3-A0FD-04546F0965F5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7554C1F3-3421-4DA4-9E82-AA5EB7A3FE84}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="1" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="4"/>
+    <tableColumn id="3" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="5" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="1"/>
+    <tableColumn id="6" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1204,23 +1618,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A190E3-387E-4B01-9613-63DEDBC60C02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.375" customWidth="1"/>
-    <col min="2" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="60.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1260,7 +1674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
@@ -1280,7 +1694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
@@ -1300,7 +1714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
@@ -1320,7 +1734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>26</v>
       </c>
@@ -1340,7 +1754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1360,7 +1774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>34</v>
       </c>
@@ -1380,7 +1794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>37</v>
       </c>
@@ -1400,7 +1814,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
@@ -1420,7 +1834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>45</v>
       </c>
@@ -1440,7 +1854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>48</v>
       </c>
@@ -1460,7 +1874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>51</v>
       </c>
@@ -1480,7 +1894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>54</v>
       </c>
@@ -1500,7 +1914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>57</v>
       </c>
@@ -1520,7 +1934,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>62</v>
       </c>
@@ -1540,7 +1954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>65</v>
       </c>
@@ -1560,7 +1974,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>70</v>
       </c>
@@ -1580,7 +1994,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>75</v>
       </c>
@@ -1600,7 +2014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>78</v>
       </c>
@@ -1620,7 +2034,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>83</v>
       </c>
@@ -1640,7 +2054,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>88</v>
       </c>
@@ -1660,7 +2074,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>93</v>
       </c>
@@ -1680,7 +2094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>96</v>
       </c>
@@ -1700,7 +2114,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
         <v>99</v>
       </c>
@@ -1720,7 +2134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>102</v>
       </c>
@@ -1740,7 +2154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>105</v>
       </c>
@@ -1760,7 +2174,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>110</v>
       </c>
@@ -1780,7 +2194,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>115</v>
       </c>
@@ -1800,7 +2214,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
         <v>120</v>
       </c>
@@ -1820,13 +2234,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" s="18"/>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G35" s="19"/>
     </row>
   </sheetData>
@@ -1840,15 +2254,2629 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9182E6F1-80B9-420E-B0AA-287A85B6DF54}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="B77:H77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>521</v>
+      </c>
+      <c r="D3" s="35">
+        <v>2.390895</v>
+      </c>
+      <c r="E3" s="2">
+        <v>11023</v>
+      </c>
+      <c r="F3" s="40">
+        <v>50.585104000000001</v>
+      </c>
+      <c r="G3" s="29">
+        <v>1572</v>
+      </c>
+      <c r="H3" s="30">
+        <v>3163</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="20">
+        <v>2</v>
+      </c>
+      <c r="C4" s="20">
+        <v>318</v>
+      </c>
+      <c r="D4" s="36">
+        <v>1.4593179999999999</v>
+      </c>
+      <c r="E4" s="20">
+        <v>8579</v>
+      </c>
+      <c r="F4" s="41">
+        <v>39.369464000000001</v>
+      </c>
+      <c r="G4" s="21">
+        <v>1242</v>
+      </c>
+      <c r="H4" s="22">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="20">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20">
+        <v>193</v>
+      </c>
+      <c r="D5" s="36">
+        <v>0.885687</v>
+      </c>
+      <c r="E5" s="20">
+        <v>6813</v>
+      </c>
+      <c r="F5" s="41">
+        <v>31.265201000000001</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1006</v>
+      </c>
+      <c r="H5" s="22">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="20">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20">
+        <v>137</v>
+      </c>
+      <c r="D6" s="36">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="E6" s="20">
+        <v>5580</v>
+      </c>
+      <c r="F6" s="41">
+        <v>25.606901999999899</v>
+      </c>
+      <c r="G6" s="21">
+        <v>849</v>
+      </c>
+      <c r="H6" s="22">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="20">
+        <v>5</v>
+      </c>
+      <c r="C7" s="20">
+        <v>103</v>
+      </c>
+      <c r="D7" s="36">
+        <v>0.47267199999999998</v>
+      </c>
+      <c r="E7" s="20">
+        <v>4304</v>
+      </c>
+      <c r="F7" s="41">
+        <v>19.751273000000001</v>
+      </c>
+      <c r="G7" s="21">
+        <v>731</v>
+      </c>
+      <c r="H7" s="22">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="20">
+        <v>6</v>
+      </c>
+      <c r="C8" s="20">
+        <v>76</v>
+      </c>
+      <c r="D8" s="36">
+        <v>0.34876799999999902</v>
+      </c>
+      <c r="E8" s="20">
+        <v>3530</v>
+      </c>
+      <c r="F8" s="41">
+        <v>16.199348000000001</v>
+      </c>
+      <c r="G8" s="21">
+        <v>642</v>
+      </c>
+      <c r="H8" s="22">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="20">
+        <v>7</v>
+      </c>
+      <c r="C9" s="20">
+        <v>63</v>
+      </c>
+      <c r="D9" s="36">
+        <v>0.28910999999999998</v>
+      </c>
+      <c r="E9" s="20">
+        <v>2952</v>
+      </c>
+      <c r="F9" s="41">
+        <v>13.546876999999901</v>
+      </c>
+      <c r="G9" s="21">
+        <v>575</v>
+      </c>
+      <c r="H9" s="22">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="20">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20">
+        <v>53</v>
+      </c>
+      <c r="D10" s="36">
+        <v>0.24321999999999999</v>
+      </c>
+      <c r="E10" s="20">
+        <v>2555</v>
+      </c>
+      <c r="F10" s="41">
+        <v>11.725023999999999</v>
+      </c>
+      <c r="G10" s="21">
+        <v>520</v>
+      </c>
+      <c r="H10" s="22">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="26">
+        <v>9</v>
+      </c>
+      <c r="C11" s="26">
+        <v>33</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.15143899999999999</v>
+      </c>
+      <c r="E11" s="26">
+        <v>2210</v>
+      </c>
+      <c r="F11" s="42">
+        <v>10.141802</v>
+      </c>
+      <c r="G11" s="27">
+        <v>469</v>
+      </c>
+      <c r="H11" s="28">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="46">
+        <v>10</v>
+      </c>
+      <c r="C12" s="32">
+        <v>27</v>
+      </c>
+      <c r="D12" s="38">
+        <v>0.123904</v>
+      </c>
+      <c r="E12" s="32">
+        <v>1919</v>
+      </c>
+      <c r="F12" s="43">
+        <v>8.8063880000000001</v>
+      </c>
+      <c r="G12" s="33">
+        <v>426</v>
+      </c>
+      <c r="H12" s="34">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>22</v>
+      </c>
+      <c r="D13" s="35">
+        <v>0.10095899999999999</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1687</v>
+      </c>
+      <c r="F13" s="40">
+        <v>7.7417280000000002</v>
+      </c>
+      <c r="G13" s="29">
+        <v>390</v>
+      </c>
+      <c r="H13" s="30">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="20">
+        <v>12</v>
+      </c>
+      <c r="C14" s="20">
+        <v>22</v>
+      </c>
+      <c r="D14" s="36">
+        <v>0.10095899999999999</v>
+      </c>
+      <c r="E14" s="20">
+        <v>1481</v>
+      </c>
+      <c r="F14" s="41">
+        <v>6.7963839999999998</v>
+      </c>
+      <c r="G14" s="21">
+        <v>360</v>
+      </c>
+      <c r="H14" s="22">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="20">
+        <v>13</v>
+      </c>
+      <c r="C15" s="20">
+        <v>21</v>
+      </c>
+      <c r="D15" s="36">
+        <v>9.6369999999999997E-2</v>
+      </c>
+      <c r="E15" s="20">
+        <v>1324</v>
+      </c>
+      <c r="F15" s="41">
+        <v>6.0759030000000003</v>
+      </c>
+      <c r="G15" s="21">
+        <v>334</v>
+      </c>
+      <c r="H15" s="22">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="20">
+        <v>14</v>
+      </c>
+      <c r="C16" s="20">
+        <v>19</v>
+      </c>
+      <c r="D16" s="36">
+        <v>8.7191999999999895E-2</v>
+      </c>
+      <c r="E16" s="20">
+        <v>1178</v>
+      </c>
+      <c r="F16" s="41">
+        <v>5.4059019999999904</v>
+      </c>
+      <c r="G16" s="21">
+        <v>312</v>
+      </c>
+      <c r="H16" s="22">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="20">
+        <v>15</v>
+      </c>
+      <c r="C17" s="20">
+        <v>16</v>
+      </c>
+      <c r="D17" s="36">
+        <v>7.3425000000000004E-2</v>
+      </c>
+      <c r="E17" s="20">
+        <v>1050</v>
+      </c>
+      <c r="F17" s="41">
+        <v>4.8185029999999998</v>
+      </c>
+      <c r="G17" s="21">
+        <v>292</v>
+      </c>
+      <c r="H17" s="22">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="20">
+        <v>16</v>
+      </c>
+      <c r="C18" s="20">
+        <v>12</v>
+      </c>
+      <c r="D18" s="36">
+        <v>5.5069E-2</v>
+      </c>
+      <c r="E18" s="20">
+        <v>942</v>
+      </c>
+      <c r="F18" s="41">
+        <v>4.3228859999999996</v>
+      </c>
+      <c r="G18" s="21">
+        <v>275</v>
+      </c>
+      <c r="H18" s="22">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="20">
+        <v>17</v>
+      </c>
+      <c r="C19" s="20">
+        <v>11</v>
+      </c>
+      <c r="D19" s="36">
+        <v>5.0479999999999997E-2</v>
+      </c>
+      <c r="E19" s="20">
+        <v>838</v>
+      </c>
+      <c r="F19" s="41">
+        <v>3.8456239999999999</v>
+      </c>
+      <c r="G19" s="21">
+        <v>259</v>
+      </c>
+      <c r="H19" s="22">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="20">
+        <v>18</v>
+      </c>
+      <c r="C20" s="20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="36">
+        <v>4.5891000000000001E-2</v>
+      </c>
+      <c r="E20" s="20">
+        <v>765</v>
+      </c>
+      <c r="F20" s="41">
+        <v>3.510624</v>
+      </c>
+      <c r="G20" s="21">
+        <v>245</v>
+      </c>
+      <c r="H20" s="22">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="20">
+        <v>19</v>
+      </c>
+      <c r="C21" s="20">
+        <v>9</v>
+      </c>
+      <c r="D21" s="36">
+        <v>4.1300999999999997E-2</v>
+      </c>
+      <c r="E21" s="20">
+        <v>687</v>
+      </c>
+      <c r="F21" s="41">
+        <v>3.1526779999999999</v>
+      </c>
+      <c r="G21" s="21">
+        <v>233</v>
+      </c>
+      <c r="H21" s="22">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="20">
+        <v>20</v>
+      </c>
+      <c r="C22" s="20">
+        <v>6</v>
+      </c>
+      <c r="D22" s="36">
+        <v>2.7533999999999899E-2</v>
+      </c>
+      <c r="E22" s="20">
+        <v>628</v>
+      </c>
+      <c r="F22" s="41">
+        <v>2.8819240000000002</v>
+      </c>
+      <c r="G22" s="21">
+        <v>222</v>
+      </c>
+      <c r="H22" s="22">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="20">
+        <v>21</v>
+      </c>
+      <c r="C23" s="20">
+        <v>6</v>
+      </c>
+      <c r="D23" s="36">
+        <v>2.7533999999999899E-2</v>
+      </c>
+      <c r="E23" s="20">
+        <v>583</v>
+      </c>
+      <c r="F23" s="41">
+        <v>2.6754159999999998</v>
+      </c>
+      <c r="G23" s="21">
+        <v>212</v>
+      </c>
+      <c r="H23" s="22">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="20">
+        <v>22</v>
+      </c>
+      <c r="C24" s="20">
+        <v>5</v>
+      </c>
+      <c r="D24" s="36">
+        <v>2.2945E-2</v>
+      </c>
+      <c r="E24" s="20">
+        <v>522</v>
+      </c>
+      <c r="F24" s="41">
+        <v>2.3954840000000002</v>
+      </c>
+      <c r="G24" s="21">
+        <v>202</v>
+      </c>
+      <c r="H24" s="22">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="20">
+        <v>23</v>
+      </c>
+      <c r="C25" s="20">
+        <v>5</v>
+      </c>
+      <c r="D25" s="36">
+        <v>2.2945E-2</v>
+      </c>
+      <c r="E25" s="20">
+        <v>487</v>
+      </c>
+      <c r="F25" s="41">
+        <v>2.2348680000000001</v>
+      </c>
+      <c r="G25" s="21">
+        <v>194</v>
+      </c>
+      <c r="H25" s="22">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="20">
+        <v>24</v>
+      </c>
+      <c r="C26" s="20">
+        <v>5</v>
+      </c>
+      <c r="D26" s="36">
+        <v>2.2945E-2</v>
+      </c>
+      <c r="E26" s="20">
+        <v>438</v>
+      </c>
+      <c r="F26" s="41">
+        <v>2.0100039999999999</v>
+      </c>
+      <c r="G26" s="21">
+        <v>186</v>
+      </c>
+      <c r="H26" s="22">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="20">
+        <v>25</v>
+      </c>
+      <c r="C27" s="20">
+        <v>4</v>
+      </c>
+      <c r="D27" s="36">
+        <v>1.8356000000000001E-2</v>
+      </c>
+      <c r="E27" s="20">
+        <v>404</v>
+      </c>
+      <c r="F27" s="41">
+        <v>1.8539759999999901</v>
+      </c>
+      <c r="G27" s="21">
+        <v>179</v>
+      </c>
+      <c r="H27" s="22">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="20">
+        <v>26</v>
+      </c>
+      <c r="C28" s="20">
+        <v>4</v>
+      </c>
+      <c r="D28" s="36">
+        <v>1.8356000000000001E-2</v>
+      </c>
+      <c r="E28" s="20">
+        <v>379</v>
+      </c>
+      <c r="F28" s="41">
+        <v>1.73925</v>
+      </c>
+      <c r="G28" s="21">
+        <v>172</v>
+      </c>
+      <c r="H28" s="22">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="20">
+        <v>27</v>
+      </c>
+      <c r="C29" s="20">
+        <v>4</v>
+      </c>
+      <c r="D29" s="36">
+        <v>1.8356000000000001E-2</v>
+      </c>
+      <c r="E29" s="20">
+        <v>353</v>
+      </c>
+      <c r="F29" s="41">
+        <v>1.6199349999999999</v>
+      </c>
+      <c r="G29" s="21">
+        <v>166</v>
+      </c>
+      <c r="H29" s="22">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="20">
+        <v>28</v>
+      </c>
+      <c r="C30" s="20">
+        <v>4</v>
+      </c>
+      <c r="D30" s="36">
+        <v>1.8356000000000001E-2</v>
+      </c>
+      <c r="E30" s="20">
+        <v>332</v>
+      </c>
+      <c r="F30" s="41">
+        <v>1.5235650000000001</v>
+      </c>
+      <c r="G30" s="21">
+        <v>160</v>
+      </c>
+      <c r="H30" s="22">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="20">
+        <v>29</v>
+      </c>
+      <c r="C31" s="20">
+        <v>2</v>
+      </c>
+      <c r="D31" s="36">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E31" s="20">
+        <v>301</v>
+      </c>
+      <c r="F31" s="41">
+        <v>1.3813040000000001</v>
+      </c>
+      <c r="G31" s="21">
+        <v>155</v>
+      </c>
+      <c r="H31" s="22">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="20">
+        <v>30</v>
+      </c>
+      <c r="C32" s="20">
+        <v>2</v>
+      </c>
+      <c r="D32" s="36">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E32" s="20">
+        <v>276</v>
+      </c>
+      <c r="F32" s="41">
+        <v>1.266578</v>
+      </c>
+      <c r="G32" s="21">
+        <v>150</v>
+      </c>
+      <c r="H32" s="22">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="20">
+        <v>31</v>
+      </c>
+      <c r="C33" s="20">
+        <v>2</v>
+      </c>
+      <c r="D33" s="36">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E33" s="20">
+        <v>263</v>
+      </c>
+      <c r="F33" s="41">
+        <v>1.20692</v>
+      </c>
+      <c r="G33" s="21">
+        <v>145</v>
+      </c>
+      <c r="H33" s="22">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="20">
+        <v>32</v>
+      </c>
+      <c r="C34" s="20">
+        <v>2</v>
+      </c>
+      <c r="D34" s="36">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E34" s="20">
+        <v>241</v>
+      </c>
+      <c r="F34" s="41">
+        <v>1.105961</v>
+      </c>
+      <c r="G34" s="21">
+        <v>140</v>
+      </c>
+      <c r="H34" s="22">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="20">
+        <v>33</v>
+      </c>
+      <c r="C35" s="20">
+        <v>2</v>
+      </c>
+      <c r="D35" s="36">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E35" s="20">
+        <v>228</v>
+      </c>
+      <c r="F35" s="41">
+        <v>1.0463039999999999</v>
+      </c>
+      <c r="G35" s="21">
+        <v>136</v>
+      </c>
+      <c r="H35" s="22">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="26">
+        <v>34</v>
+      </c>
+      <c r="C36" s="26">
+        <v>2</v>
+      </c>
+      <c r="D36" s="37">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="E36" s="26">
+        <v>210</v>
+      </c>
+      <c r="F36" s="42">
+        <v>0.96370100000000003</v>
+      </c>
+      <c r="G36" s="27">
+        <v>132</v>
+      </c>
+      <c r="H36" s="28">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="45">
+        <v>35</v>
+      </c>
+      <c r="C37" s="32">
+        <v>1</v>
+      </c>
+      <c r="D37" s="38">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E37" s="32">
+        <v>194</v>
+      </c>
+      <c r="F37" s="43">
+        <v>0.89027599999999996</v>
+      </c>
+      <c r="G37" s="33">
+        <v>128</v>
+      </c>
+      <c r="H37" s="34">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="35">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E38" s="2">
+        <v>184</v>
+      </c>
+      <c r="F38" s="40">
+        <v>0.84438500000000005</v>
+      </c>
+      <c r="G38" s="29">
+        <v>125</v>
+      </c>
+      <c r="H38" s="30">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="20">
+        <v>37</v>
+      </c>
+      <c r="C39" s="20">
+        <v>1</v>
+      </c>
+      <c r="D39" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E39" s="20">
+        <v>174</v>
+      </c>
+      <c r="F39" s="41">
+        <v>0.79849499999999995</v>
+      </c>
+      <c r="G39" s="21">
+        <v>122</v>
+      </c>
+      <c r="H39" s="22">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="20">
+        <v>38</v>
+      </c>
+      <c r="C40" s="20">
+        <v>1</v>
+      </c>
+      <c r="D40" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E40" s="20">
+        <v>164</v>
+      </c>
+      <c r="F40" s="41">
+        <v>0.75260400000000005</v>
+      </c>
+      <c r="G40" s="21">
+        <v>118</v>
+      </c>
+      <c r="H40" s="22">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="20">
+        <v>39</v>
+      </c>
+      <c r="C41" s="20">
+        <v>1</v>
+      </c>
+      <c r="D41" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E41" s="20">
+        <v>159</v>
+      </c>
+      <c r="F41" s="41">
+        <v>0.72965899999999995</v>
+      </c>
+      <c r="G41" s="21">
+        <v>115</v>
+      </c>
+      <c r="H41" s="22">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="20">
+        <v>40</v>
+      </c>
+      <c r="C42" s="20">
+        <v>1</v>
+      </c>
+      <c r="D42" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E42" s="20">
+        <v>143</v>
+      </c>
+      <c r="F42" s="41">
+        <v>0.65623399999999998</v>
+      </c>
+      <c r="G42" s="21">
+        <v>112</v>
+      </c>
+      <c r="H42" s="22">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="20">
+        <v>41</v>
+      </c>
+      <c r="C43" s="20">
+        <v>1</v>
+      </c>
+      <c r="D43" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E43" s="20">
+        <v>133</v>
+      </c>
+      <c r="F43" s="41">
+        <v>0.610344</v>
+      </c>
+      <c r="G43" s="21">
+        <v>110</v>
+      </c>
+      <c r="H43" s="22">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="20">
+        <v>42</v>
+      </c>
+      <c r="C44" s="20">
+        <v>1</v>
+      </c>
+      <c r="D44" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E44" s="20">
+        <v>127</v>
+      </c>
+      <c r="F44" s="41">
+        <v>0.58280900000000002</v>
+      </c>
+      <c r="G44" s="21">
+        <v>107</v>
+      </c>
+      <c r="H44" s="22">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="20">
+        <v>43</v>
+      </c>
+      <c r="C45" s="20">
+        <v>1</v>
+      </c>
+      <c r="D45" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E45" s="20">
+        <v>117</v>
+      </c>
+      <c r="F45" s="41">
+        <v>0.53691899999999904</v>
+      </c>
+      <c r="G45" s="21">
+        <v>105</v>
+      </c>
+      <c r="H45" s="22">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="20">
+        <v>44</v>
+      </c>
+      <c r="C46" s="20">
+        <v>1</v>
+      </c>
+      <c r="D46" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E46" s="20">
+        <v>112</v>
+      </c>
+      <c r="F46" s="41">
+        <v>0.51397399999999904</v>
+      </c>
+      <c r="G46" s="21">
+        <v>102</v>
+      </c>
+      <c r="H46" s="22">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="20">
+        <v>45</v>
+      </c>
+      <c r="C47" s="20">
+        <v>1</v>
+      </c>
+      <c r="D47" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E47" s="20">
+        <v>107</v>
+      </c>
+      <c r="F47" s="41">
+        <v>0.49102799999999902</v>
+      </c>
+      <c r="G47" s="21">
+        <v>100</v>
+      </c>
+      <c r="H47" s="22">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="20">
+        <v>46</v>
+      </c>
+      <c r="C48" s="20">
+        <v>1</v>
+      </c>
+      <c r="D48" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E48" s="20">
+        <v>103</v>
+      </c>
+      <c r="F48" s="41">
+        <v>0.47267199999999998</v>
+      </c>
+      <c r="G48" s="21">
+        <v>98</v>
+      </c>
+      <c r="H48" s="22">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="20">
+        <v>47</v>
+      </c>
+      <c r="C49" s="20">
+        <v>1</v>
+      </c>
+      <c r="D49" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E49" s="20">
+        <v>96</v>
+      </c>
+      <c r="F49" s="41">
+        <v>0.44054899999999902</v>
+      </c>
+      <c r="G49" s="21">
+        <v>96</v>
+      </c>
+      <c r="H49" s="22">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="20">
+        <v>48</v>
+      </c>
+      <c r="C50" s="20">
+        <v>1</v>
+      </c>
+      <c r="D50" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E50" s="20">
+        <v>94</v>
+      </c>
+      <c r="F50" s="41">
+        <v>0.431371</v>
+      </c>
+      <c r="G50" s="21">
+        <v>94</v>
+      </c>
+      <c r="H50" s="22">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="20">
+        <v>49</v>
+      </c>
+      <c r="C51" s="20">
+        <v>1</v>
+      </c>
+      <c r="D51" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E51" s="20">
+        <v>85</v>
+      </c>
+      <c r="F51" s="41">
+        <v>0.390069</v>
+      </c>
+      <c r="G51" s="21">
+        <v>92</v>
+      </c>
+      <c r="H51" s="22">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="20">
+        <v>50</v>
+      </c>
+      <c r="C52" s="20">
+        <v>1</v>
+      </c>
+      <c r="D52" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E52" s="20">
+        <v>84</v>
+      </c>
+      <c r="F52" s="41">
+        <v>0.38547999999999999</v>
+      </c>
+      <c r="G52" s="21">
+        <v>90</v>
+      </c>
+      <c r="H52" s="22">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="20">
+        <v>51</v>
+      </c>
+      <c r="C53" s="20">
+        <v>1</v>
+      </c>
+      <c r="D53" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E53" s="20">
+        <v>82</v>
+      </c>
+      <c r="F53" s="41">
+        <v>0.37630200000000003</v>
+      </c>
+      <c r="G53" s="21">
+        <v>88</v>
+      </c>
+      <c r="H53" s="22">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="20">
+        <v>52</v>
+      </c>
+      <c r="C54" s="20">
+        <v>1</v>
+      </c>
+      <c r="D54" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E54" s="20">
+        <v>80</v>
+      </c>
+      <c r="F54" s="41">
+        <v>0.36712400000000001</v>
+      </c>
+      <c r="G54" s="21">
+        <v>86</v>
+      </c>
+      <c r="H54" s="22">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="20">
+        <v>53</v>
+      </c>
+      <c r="C55" s="20">
+        <v>1</v>
+      </c>
+      <c r="D55" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E55" s="20">
+        <v>75</v>
+      </c>
+      <c r="F55" s="41">
+        <v>0.34417900000000001</v>
+      </c>
+      <c r="G55" s="21">
+        <v>85</v>
+      </c>
+      <c r="H55" s="22">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="20">
+        <v>54</v>
+      </c>
+      <c r="C56" s="20">
+        <v>1</v>
+      </c>
+      <c r="D56" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E56" s="20">
+        <v>70</v>
+      </c>
+      <c r="F56" s="41">
+        <v>0.32123400000000002</v>
+      </c>
+      <c r="G56" s="21">
+        <v>83</v>
+      </c>
+      <c r="H56" s="22">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="20">
+        <v>55</v>
+      </c>
+      <c r="C57" s="20">
+        <v>1</v>
+      </c>
+      <c r="D57" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E57" s="20">
+        <v>66</v>
+      </c>
+      <c r="F57" s="41">
+        <v>0.30287700000000001</v>
+      </c>
+      <c r="G57" s="21">
+        <v>82</v>
+      </c>
+      <c r="H57" s="22">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="20">
+        <v>56</v>
+      </c>
+      <c r="C58" s="20">
+        <v>1</v>
+      </c>
+      <c r="D58" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E58" s="20">
+        <v>58</v>
+      </c>
+      <c r="F58" s="41">
+        <v>0.26616499999999998</v>
+      </c>
+      <c r="G58" s="21">
+        <v>80</v>
+      </c>
+      <c r="H58" s="22">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="20">
+        <v>57</v>
+      </c>
+      <c r="C59" s="20">
+        <v>1</v>
+      </c>
+      <c r="D59" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E59" s="20">
+        <v>58</v>
+      </c>
+      <c r="F59" s="41">
+        <v>0.26616499999999998</v>
+      </c>
+      <c r="G59" s="21">
+        <v>79</v>
+      </c>
+      <c r="H59" s="22">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="20">
+        <v>58</v>
+      </c>
+      <c r="C60" s="20">
+        <v>1</v>
+      </c>
+      <c r="D60" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E60" s="20">
+        <v>52</v>
+      </c>
+      <c r="F60" s="41">
+        <v>0.23863099999999901</v>
+      </c>
+      <c r="G60" s="21">
+        <v>77</v>
+      </c>
+      <c r="H60" s="22">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="20">
+        <v>59</v>
+      </c>
+      <c r="C61" s="20">
+        <v>1</v>
+      </c>
+      <c r="D61" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E61" s="20">
+        <v>51</v>
+      </c>
+      <c r="F61" s="41">
+        <v>0.234042</v>
+      </c>
+      <c r="G61" s="21">
+        <v>76</v>
+      </c>
+      <c r="H61" s="22">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="20">
+        <v>60</v>
+      </c>
+      <c r="C62" s="20">
+        <v>1</v>
+      </c>
+      <c r="D62" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E62" s="20">
+        <v>49</v>
+      </c>
+      <c r="F62" s="41">
+        <v>0.22486300000000001</v>
+      </c>
+      <c r="G62" s="21">
+        <v>75</v>
+      </c>
+      <c r="H62" s="22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="20">
+        <v>61</v>
+      </c>
+      <c r="C63" s="20">
+        <v>1</v>
+      </c>
+      <c r="D63" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E63" s="20">
+        <v>47</v>
+      </c>
+      <c r="F63" s="41">
+        <v>0.21568499999999999</v>
+      </c>
+      <c r="G63" s="21">
+        <v>74</v>
+      </c>
+      <c r="H63" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="20">
+        <v>62</v>
+      </c>
+      <c r="C64" s="20">
+        <v>1</v>
+      </c>
+      <c r="D64" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E64" s="20">
+        <v>46</v>
+      </c>
+      <c r="F64" s="41">
+        <v>0.21109600000000001</v>
+      </c>
+      <c r="G64" s="21">
+        <v>72</v>
+      </c>
+      <c r="H64" s="22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="20">
+        <v>63</v>
+      </c>
+      <c r="C65" s="20">
+        <v>1</v>
+      </c>
+      <c r="D65" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E65" s="20">
+        <v>45</v>
+      </c>
+      <c r="F65" s="41">
+        <v>0.206507</v>
+      </c>
+      <c r="G65" s="21">
+        <v>71</v>
+      </c>
+      <c r="H65" s="22">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="20">
+        <v>64</v>
+      </c>
+      <c r="C66" s="20">
+        <v>1</v>
+      </c>
+      <c r="D66" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E66" s="20">
+        <v>43</v>
+      </c>
+      <c r="F66" s="41">
+        <v>0.197329</v>
+      </c>
+      <c r="G66" s="21">
+        <v>70</v>
+      </c>
+      <c r="H66" s="22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="20">
+        <v>65</v>
+      </c>
+      <c r="C67" s="20">
+        <v>1</v>
+      </c>
+      <c r="D67" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E67" s="20">
+        <v>40</v>
+      </c>
+      <c r="F67" s="41">
+        <v>0.183562</v>
+      </c>
+      <c r="G67" s="21">
+        <v>69</v>
+      </c>
+      <c r="H67" s="22">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="20">
+        <v>66</v>
+      </c>
+      <c r="C68" s="20">
+        <v>1</v>
+      </c>
+      <c r="D68" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E68" s="20">
+        <v>37</v>
+      </c>
+      <c r="F68" s="41">
+        <v>0.169795</v>
+      </c>
+      <c r="G68" s="21">
+        <v>68</v>
+      </c>
+      <c r="H68" s="22">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="20">
+        <v>67</v>
+      </c>
+      <c r="C69" s="20">
+        <v>1</v>
+      </c>
+      <c r="D69" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E69" s="20">
+        <v>37</v>
+      </c>
+      <c r="F69" s="41">
+        <v>0.169795</v>
+      </c>
+      <c r="G69" s="21">
+        <v>67</v>
+      </c>
+      <c r="H69" s="22">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="20">
+        <v>68</v>
+      </c>
+      <c r="C70" s="20">
+        <v>1</v>
+      </c>
+      <c r="D70" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E70" s="20">
+        <v>37</v>
+      </c>
+      <c r="F70" s="41">
+        <v>0.169795</v>
+      </c>
+      <c r="G70" s="21">
+        <v>66</v>
+      </c>
+      <c r="H70" s="22">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="20">
+        <v>69</v>
+      </c>
+      <c r="C71" s="20">
+        <v>1</v>
+      </c>
+      <c r="D71" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E71" s="20">
+        <v>36</v>
+      </c>
+      <c r="F71" s="41">
+        <v>0.16520599999999999</v>
+      </c>
+      <c r="G71" s="21">
+        <v>65</v>
+      </c>
+      <c r="H71" s="22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="20">
+        <v>70</v>
+      </c>
+      <c r="C72" s="20">
+        <v>1</v>
+      </c>
+      <c r="D72" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E72" s="20">
+        <v>36</v>
+      </c>
+      <c r="F72" s="41">
+        <v>0.16520599999999999</v>
+      </c>
+      <c r="G72" s="21">
+        <v>64</v>
+      </c>
+      <c r="H72" s="22">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="20">
+        <v>71</v>
+      </c>
+      <c r="C73" s="20">
+        <v>1</v>
+      </c>
+      <c r="D73" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E73" s="20">
+        <v>36</v>
+      </c>
+      <c r="F73" s="41">
+        <v>0.16520599999999999</v>
+      </c>
+      <c r="G73" s="21">
+        <v>63</v>
+      </c>
+      <c r="H73" s="22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="26">
+        <v>72</v>
+      </c>
+      <c r="C74" s="26">
+        <v>1</v>
+      </c>
+      <c r="D74" s="37">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E74" s="26">
+        <v>36</v>
+      </c>
+      <c r="F74" s="42">
+        <v>0.16520599999999999</v>
+      </c>
+      <c r="G74" s="27">
+        <v>62</v>
+      </c>
+      <c r="H74" s="28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="46">
+        <v>73</v>
+      </c>
+      <c r="C75" s="32">
+        <v>1</v>
+      </c>
+      <c r="D75" s="38">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E75" s="32">
+        <v>34</v>
+      </c>
+      <c r="F75" s="43">
+        <v>0.156028</v>
+      </c>
+      <c r="G75" s="33">
+        <v>61</v>
+      </c>
+      <c r="H75" s="34">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>74</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="35">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E76" s="2">
+        <v>32</v>
+      </c>
+      <c r="F76" s="40">
+        <v>0.14685000000000001</v>
+      </c>
+      <c r="G76" s="29">
+        <v>60</v>
+      </c>
+      <c r="H76" s="30">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="20">
+        <v>75</v>
+      </c>
+      <c r="C77" s="20">
+        <v>1</v>
+      </c>
+      <c r="D77" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E77" s="20">
+        <v>29</v>
+      </c>
+      <c r="F77" s="41">
+        <v>0.13308200000000001</v>
+      </c>
+      <c r="G77" s="21">
+        <v>60</v>
+      </c>
+      <c r="H77" s="22">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="23">
+        <v>76</v>
+      </c>
+      <c r="C78" s="23">
+        <v>1</v>
+      </c>
+      <c r="D78" s="39">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E78" s="23">
+        <v>26</v>
+      </c>
+      <c r="F78" s="44">
+        <v>0.119315</v>
+      </c>
+      <c r="G78" s="24">
+        <v>59</v>
+      </c>
+      <c r="H78" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="20">
+        <v>77</v>
+      </c>
+      <c r="C79" s="20">
+        <v>1</v>
+      </c>
+      <c r="D79" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E79" s="20">
+        <v>25</v>
+      </c>
+      <c r="F79" s="41">
+        <v>0.11472599999999999</v>
+      </c>
+      <c r="G79" s="21">
+        <v>58</v>
+      </c>
+      <c r="H79" s="22">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="20">
+        <v>78</v>
+      </c>
+      <c r="C80" s="20">
+        <v>1</v>
+      </c>
+      <c r="D80" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E80" s="20">
+        <v>24</v>
+      </c>
+      <c r="F80" s="41">
+        <v>0.110136999999999</v>
+      </c>
+      <c r="G80" s="21">
+        <v>57</v>
+      </c>
+      <c r="H80" s="22">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="20">
+        <v>79</v>
+      </c>
+      <c r="C81" s="20">
+        <v>1</v>
+      </c>
+      <c r="D81" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E81" s="20">
+        <v>24</v>
+      </c>
+      <c r="F81" s="41">
+        <v>0.110136999999999</v>
+      </c>
+      <c r="G81" s="21">
+        <v>56</v>
+      </c>
+      <c r="H81" s="22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="20">
+        <v>80</v>
+      </c>
+      <c r="C82" s="20">
+        <v>1</v>
+      </c>
+      <c r="D82" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E82" s="20">
+        <v>24</v>
+      </c>
+      <c r="F82" s="41">
+        <v>0.110136999999999</v>
+      </c>
+      <c r="G82" s="21">
+        <v>56</v>
+      </c>
+      <c r="H82" s="22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="20">
+        <v>81</v>
+      </c>
+      <c r="C83" s="20">
+        <v>1</v>
+      </c>
+      <c r="D83" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E83" s="20">
+        <v>22</v>
+      </c>
+      <c r="F83" s="41">
+        <v>0.10095899999999999</v>
+      </c>
+      <c r="G83" s="21">
+        <v>55</v>
+      </c>
+      <c r="H83" s="22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="20">
+        <v>82</v>
+      </c>
+      <c r="C84" s="20">
+        <v>1</v>
+      </c>
+      <c r="D84" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E84" s="20">
+        <v>20</v>
+      </c>
+      <c r="F84" s="41">
+        <v>9.1781000000000001E-2</v>
+      </c>
+      <c r="G84" s="21">
+        <v>54</v>
+      </c>
+      <c r="H84" s="22">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="20">
+        <v>83</v>
+      </c>
+      <c r="C85" s="20">
+        <v>1</v>
+      </c>
+      <c r="D85" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E85" s="20">
+        <v>20</v>
+      </c>
+      <c r="F85" s="41">
+        <v>9.1781000000000001E-2</v>
+      </c>
+      <c r="G85" s="21">
+        <v>54</v>
+      </c>
+      <c r="H85" s="22">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="20">
+        <v>84</v>
+      </c>
+      <c r="C86" s="20">
+        <v>1</v>
+      </c>
+      <c r="D86" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E86" s="20">
+        <v>19</v>
+      </c>
+      <c r="F86" s="41">
+        <v>8.7191999999999895E-2</v>
+      </c>
+      <c r="G86" s="21">
+        <v>53</v>
+      </c>
+      <c r="H86" s="22">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="20">
+        <v>85</v>
+      </c>
+      <c r="C87" s="20">
+        <v>1</v>
+      </c>
+      <c r="D87" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E87" s="20">
+        <v>18</v>
+      </c>
+      <c r="F87" s="41">
+        <v>8.2602999999999996E-2</v>
+      </c>
+      <c r="G87" s="21">
+        <v>52</v>
+      </c>
+      <c r="H87" s="22">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="20">
+        <v>86</v>
+      </c>
+      <c r="C88" s="20">
+        <v>1</v>
+      </c>
+      <c r="D88" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E88" s="20">
+        <v>17</v>
+      </c>
+      <c r="F88" s="41">
+        <v>7.8014E-2</v>
+      </c>
+      <c r="G88" s="21">
+        <v>52</v>
+      </c>
+      <c r="H88" s="22">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="20">
+        <v>87</v>
+      </c>
+      <c r="C89" s="20">
+        <v>1</v>
+      </c>
+      <c r="D89" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E89" s="20">
+        <v>17</v>
+      </c>
+      <c r="F89" s="41">
+        <v>7.8014E-2</v>
+      </c>
+      <c r="G89" s="21">
+        <v>51</v>
+      </c>
+      <c r="H89" s="22">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="20">
+        <v>88</v>
+      </c>
+      <c r="C90" s="20">
+        <v>1</v>
+      </c>
+      <c r="D90" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E90" s="20">
+        <v>17</v>
+      </c>
+      <c r="F90" s="41">
+        <v>7.8014E-2</v>
+      </c>
+      <c r="G90" s="21">
+        <v>51</v>
+      </c>
+      <c r="H90" s="22">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="20">
+        <v>89</v>
+      </c>
+      <c r="C91" s="20">
+        <v>1</v>
+      </c>
+      <c r="D91" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E91" s="20">
+        <v>16</v>
+      </c>
+      <c r="F91" s="41">
+        <v>7.3425000000000004E-2</v>
+      </c>
+      <c r="G91" s="21">
+        <v>50</v>
+      </c>
+      <c r="H91" s="22">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="20">
+        <v>90</v>
+      </c>
+      <c r="C92" s="20">
+        <v>1</v>
+      </c>
+      <c r="D92" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E92" s="20">
+        <v>15</v>
+      </c>
+      <c r="F92" s="41">
+        <v>6.8835999999999994E-2</v>
+      </c>
+      <c r="G92" s="21">
+        <v>49</v>
+      </c>
+      <c r="H92" s="22">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="20">
+        <v>91</v>
+      </c>
+      <c r="C93" s="20">
+        <v>1</v>
+      </c>
+      <c r="D93" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E93" s="20">
+        <v>14</v>
+      </c>
+      <c r="F93" s="41">
+        <v>6.4246999999999999E-2</v>
+      </c>
+      <c r="G93" s="21">
+        <v>49</v>
+      </c>
+      <c r="H93" s="22">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="20">
+        <v>92</v>
+      </c>
+      <c r="C94" s="20">
+        <v>1</v>
+      </c>
+      <c r="D94" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E94" s="20">
+        <v>13</v>
+      </c>
+      <c r="F94" s="41">
+        <v>5.9658000000000003E-2</v>
+      </c>
+      <c r="G94" s="21">
+        <v>48</v>
+      </c>
+      <c r="H94" s="22">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="20">
+        <v>93</v>
+      </c>
+      <c r="C95" s="20">
+        <v>1</v>
+      </c>
+      <c r="D95" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E95" s="20">
+        <v>13</v>
+      </c>
+      <c r="F95" s="41">
+        <v>5.9658000000000003E-2</v>
+      </c>
+      <c r="G95" s="21">
+        <v>48</v>
+      </c>
+      <c r="H95" s="22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="20">
+        <v>94</v>
+      </c>
+      <c r="C96" s="20">
+        <v>1</v>
+      </c>
+      <c r="D96" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E96" s="20">
+        <v>11</v>
+      </c>
+      <c r="F96" s="41">
+        <v>5.0479999999999997E-2</v>
+      </c>
+      <c r="G96" s="21">
+        <v>47</v>
+      </c>
+      <c r="H96" s="22">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="20">
+        <v>95</v>
+      </c>
+      <c r="C97" s="20">
+        <v>1</v>
+      </c>
+      <c r="D97" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E97" s="20">
+        <v>11</v>
+      </c>
+      <c r="F97" s="41">
+        <v>5.0479999999999997E-2</v>
+      </c>
+      <c r="G97" s="21">
+        <v>47</v>
+      </c>
+      <c r="H97" s="22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="20">
+        <v>96</v>
+      </c>
+      <c r="C98" s="20">
+        <v>1</v>
+      </c>
+      <c r="D98" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E98" s="20">
+        <v>10</v>
+      </c>
+      <c r="F98" s="41">
+        <v>4.5891000000000001E-2</v>
+      </c>
+      <c r="G98" s="21">
+        <v>46</v>
+      </c>
+      <c r="H98" s="22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="26">
+        <v>97</v>
+      </c>
+      <c r="C99" s="26">
+        <v>1</v>
+      </c>
+      <c r="D99" s="37">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E99" s="26">
+        <v>9</v>
+      </c>
+      <c r="F99" s="42">
+        <v>4.1300999999999997E-2</v>
+      </c>
+      <c r="G99" s="27">
+        <v>46</v>
+      </c>
+      <c r="H99" s="28">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="45">
+        <v>98</v>
+      </c>
+      <c r="C100" s="32">
+        <v>1</v>
+      </c>
+      <c r="D100" s="38">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E100" s="32">
+        <v>8</v>
+      </c>
+      <c r="F100" s="43">
+        <v>3.6712000000000002E-2</v>
+      </c>
+      <c r="G100" s="33">
+        <v>45</v>
+      </c>
+      <c r="H100" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="2">
+        <v>99</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1</v>
+      </c>
+      <c r="D101" s="35">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E101" s="2">
+        <v>8</v>
+      </c>
+      <c r="F101" s="40">
+        <v>3.6712000000000002E-2</v>
+      </c>
+      <c r="G101" s="29">
+        <v>45</v>
+      </c>
+      <c r="H101" s="30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="20">
+        <v>100</v>
+      </c>
+      <c r="C102" s="20">
+        <v>1</v>
+      </c>
+      <c r="D102" s="36">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="E102" s="20">
+        <v>8</v>
+      </c>
+      <c r="F102" s="41">
+        <v>3.6712000000000002E-2</v>
+      </c>
+      <c r="G102" s="21">
+        <v>44</v>
+      </c>
+      <c r="H102" s="22">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="51">
+        <v>5</v>
+      </c>
+      <c r="C3" s="53">
+        <v>0.47267199999999998</v>
+      </c>
+      <c r="D3" s="62">
+        <v>19.751273000000001</v>
+      </c>
+      <c r="E3" s="57">
+        <v>731</v>
+      </c>
+      <c r="F3" s="67">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="49">
+        <v>10</v>
+      </c>
+      <c r="C4" s="54">
+        <v>0.123904</v>
+      </c>
+      <c r="D4" s="63">
+        <v>8.8063880000000001</v>
+      </c>
+      <c r="E4" s="58">
+        <v>426</v>
+      </c>
+      <c r="F4" s="68">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="47">
+        <v>20</v>
+      </c>
+      <c r="C5" s="55">
+        <v>2.7533999999999899E-2</v>
+      </c>
+      <c r="D5" s="64">
+        <v>2.8819240000000002</v>
+      </c>
+      <c r="E5" s="59">
+        <v>222</v>
+      </c>
+      <c r="F5" s="69">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="47">
+        <v>30</v>
+      </c>
+      <c r="C6" s="55">
+        <v>9.1780000000000004E-3</v>
+      </c>
+      <c r="D6" s="64">
+        <v>1.266578</v>
+      </c>
+      <c r="E6" s="59">
+        <v>150</v>
+      </c>
+      <c r="F6" s="69">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="50">
+        <v>35</v>
+      </c>
+      <c r="C7" s="54">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D7" s="63">
+        <v>0.89027599999999996</v>
+      </c>
+      <c r="E7" s="58">
+        <v>128</v>
+      </c>
+      <c r="F7" s="68">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="47">
+        <v>40</v>
+      </c>
+      <c r="C8" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D8" s="64">
+        <v>0.65623399999999998</v>
+      </c>
+      <c r="E8" s="59">
+        <v>112</v>
+      </c>
+      <c r="F8" s="69">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="47">
+        <v>50</v>
+      </c>
+      <c r="C9" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D9" s="64">
+        <v>0.38547999999999999</v>
+      </c>
+      <c r="E9" s="59">
+        <v>90</v>
+      </c>
+      <c r="F9" s="69">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="47">
+        <v>60</v>
+      </c>
+      <c r="C10" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D10" s="64">
+        <v>0.22486300000000001</v>
+      </c>
+      <c r="E10" s="59">
+        <v>75</v>
+      </c>
+      <c r="F10" s="69">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="47">
+        <v>70</v>
+      </c>
+      <c r="C11" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D11" s="64">
+        <v>0.16520599999999999</v>
+      </c>
+      <c r="E11" s="59">
+        <v>64</v>
+      </c>
+      <c r="F11" s="69">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="49">
+        <v>75</v>
+      </c>
+      <c r="C12" s="54">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D12" s="63">
+        <v>0.13308200000000001</v>
+      </c>
+      <c r="E12" s="58">
+        <v>60</v>
+      </c>
+      <c r="F12" s="68">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="47">
+        <v>80</v>
+      </c>
+      <c r="C13" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D13" s="64">
+        <v>0.110136999999999</v>
+      </c>
+      <c r="E13" s="59">
+        <v>56</v>
+      </c>
+      <c r="F13" s="69">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="47">
+        <v>90</v>
+      </c>
+      <c r="C14" s="55">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D14" s="64">
+        <v>6.8835999999999994E-2</v>
+      </c>
+      <c r="E14" s="59">
+        <v>49</v>
+      </c>
+      <c r="F14" s="69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="50">
+        <v>98</v>
+      </c>
+      <c r="C15" s="54">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D15" s="63">
+        <v>3.6712000000000002E-2</v>
+      </c>
+      <c r="E15" s="58">
+        <v>45</v>
+      </c>
+      <c r="F15" s="68">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="48">
+        <v>100</v>
+      </c>
+      <c r="C16" s="56">
+        <v>4.5890000000000002E-3</v>
+      </c>
+      <c r="D16" s="65">
+        <v>3.6712000000000002E-2</v>
+      </c>
+      <c r="E16" s="60">
+        <v>44</v>
+      </c>
+      <c r="F16" s="70">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Merged professor's version with new figures
</commit_message>
<xml_diff>
--- a/20_Experiments/false_positive_20180214.xlsx
+++ b/20_Experiments/false_positive_20180214.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29740" yWindow="-7200" windowWidth="19820" windowHeight="19460" activeTab="2"/>
+    <workbookView xWindow="6420" yWindow="460" windowWidth="22380" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -524,7 +524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +564,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,7 +866,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1054,6 +1078,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="185" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1282,6 +1318,1130 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$5:$J$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="98"/>
+                <c:pt idx="0">
+                  <c:v>35.30050796726157</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.72992206139637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.78642483582696</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.44734608679708</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.85717201065304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48.20748293725845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.9695520968839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71.0742833161157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76.68190057350014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67.31825790667499</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.04766006018471</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.99997706211575</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65.62482805583929</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>78.49944614937622</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>76.1811410459588</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>76.49918284630974</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>76.33418077044139</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104.6678288661295</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97.16771990992988</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104.4011331444759</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>97.40108956199607</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>87.60095881455655</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>101.0010895619955</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>94.75103508389627</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>88.25098060579645</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>83.00092612769667</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>150.5016343429941</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>138.0015253867945</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>131.501416430595</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>120.5013074743953</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>114.0013074743953</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>105.0011985181957</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>194.0021791239921</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>184.0019612115929</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>174.0019612115929</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>164.0017432991937</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>159.0017432991937</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>143.0015253867945</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>133.0015253867945</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>127.0013074743953</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>117.0013074743951</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>112.0013074743951</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>107.0010895619959</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>103.0010895619961</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>96.00108956199585</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94.00108956199606</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>85.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>84.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>82.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>80.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>75.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>70.00087164959686</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>66.00065373719765</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>58.00065373719764</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>58.00065373719764</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>52.00065373719743</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>51.00065373719764</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>49.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>47.00043582479842</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>46.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>45.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>43.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>40.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>37.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>37.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>37.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>36.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>36.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>36.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>36.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>34.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>32.00043582479843</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>29.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>26.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>25.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>24.00021791239899</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>24.00021791239899</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>24.00021791239899</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>22.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>20.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>20.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>19.00021791239919</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>18.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>17.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>17.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>17.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>16.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>15.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>14.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>13.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>13.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>11.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>11.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10.00021791239921</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>8.999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2038354512"/>
+        <c:axId val="-2038352000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2038354512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2038352000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2038352000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2038354512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>194732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>211666</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1622,7 +2782,7 @@
   <dimension ref="B2:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2255,11 +3415,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H102"/>
+  <dimension ref="B1:L102"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77:H77"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2274,8 +3434,8 @@
     <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
         <v>123</v>
       </c>
@@ -2298,7 +3458,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -2320,8 +3480,16 @@
       <c r="H3" s="30">
         <v>3163</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>F3/D3</f>
+        <v>21.157392524556705</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(J3:J102)</f>
+        <v>64.024865475776366</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="20">
         <v>2</v>
       </c>
@@ -2343,8 +3511,12 @@
       <c r="H4" s="22">
         <v>2108</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" ref="J4:J67" si="0">F4/D4</f>
+        <v>26.977988347981732</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="20">
         <v>3</v>
       </c>
@@ -2366,8 +3538,12 @@
       <c r="H5" s="22">
         <v>1581</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>35.300507967261574</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="20">
         <v>4</v>
       </c>
@@ -2389,8 +3565,12 @@
       <c r="H6" s="22">
         <v>1264</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>40.729922061396366</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="20">
         <v>5</v>
       </c>
@@ -2412,8 +3592,12 @@
       <c r="H7" s="22">
         <v>1054</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>41.786424835826963</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="20">
         <v>6</v>
       </c>
@@ -2435,8 +3619,12 @@
       <c r="H8" s="22">
         <v>902</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>46.447346086797083</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="20">
         <v>7</v>
       </c>
@@ -2458,8 +3646,12 @@
       <c r="H9" s="22">
         <v>789</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>46.857172010653045</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="20">
         <v>8</v>
       </c>
@@ -2481,8 +3673,12 @@
       <c r="H10" s="22">
         <v>701</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>48.207482937258447</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26">
         <v>9</v>
       </c>
@@ -2504,8 +3700,12 @@
       <c r="H11" s="28">
         <v>631</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>66.969552096883902</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="46">
         <v>10</v>
       </c>
@@ -2527,8 +3727,12 @@
       <c r="H12" s="34">
         <v>573</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>71.074283316115697</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>11</v>
       </c>
@@ -2550,8 +3754,12 @@
       <c r="H13" s="30">
         <v>525</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>76.681900573500144</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <v>12</v>
       </c>
@@ -2573,8 +3781,12 @@
       <c r="H14" s="22">
         <v>485</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>67.318257906674987</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="20">
         <v>13</v>
       </c>
@@ -2596,8 +3808,12 @@
       <c r="H15" s="22">
         <v>450</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>63.047660060184711</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="20">
         <v>14</v>
       </c>
@@ -2619,8 +3835,12 @@
       <c r="H16" s="22">
         <v>420</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>61.999977062115754</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>15</v>
       </c>
@@ -2642,8 +3862,12 @@
       <c r="H17" s="22">
         <v>393</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>65.624828055839288</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <v>16</v>
       </c>
@@ -2665,8 +3889,12 @@
       <c r="H18" s="22">
         <v>370</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>78.499446149376226</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <v>17</v>
       </c>
@@ -2688,8 +3916,12 @@
       <c r="H19" s="22">
         <v>350</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>76.181141045958796</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <v>18</v>
       </c>
@@ -2711,8 +3943,12 @@
       <c r="H20" s="22">
         <v>331</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>76.499182846309736</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <v>19</v>
       </c>
@@ -2734,8 +3970,12 @@
       <c r="H21" s="22">
         <v>314</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>76.334180770441392</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <v>20</v>
       </c>
@@ -2757,8 +3997,12 @@
       <c r="H22" s="22">
         <v>299</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>104.66782886612954</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <v>21</v>
       </c>
@@ -2780,8 +4024,12 @@
       <c r="H23" s="22">
         <v>285</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>97.167719909929886</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <v>22</v>
       </c>
@@ -2803,8 +4051,12 @@
       <c r="H24" s="22">
         <v>273</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>104.40113314447592</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <v>23</v>
       </c>
@@ -2826,8 +4078,12 @@
       <c r="H25" s="22">
         <v>261</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>97.401089561996073</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <v>24</v>
       </c>
@@ -2849,8 +4105,12 @@
       <c r="H26" s="22">
         <v>251</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>87.600958814556549</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <v>25</v>
       </c>
@@ -2872,8 +4132,12 @@
       <c r="H27" s="22">
         <v>241</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>101.00108956199553</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <v>26</v>
       </c>
@@ -2895,8 +4159,12 @@
       <c r="H28" s="22">
         <v>232</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>94.751035083896269</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="20">
         <v>27</v>
       </c>
@@ -2918,8 +4186,12 @@
       <c r="H29" s="22">
         <v>224</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>88.250980605796457</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="20">
         <v>28</v>
       </c>
@@ -2941,8 +4213,12 @@
       <c r="H30" s="22">
         <v>216</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>83.000926127696673</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="20">
         <v>29</v>
       </c>
@@ -2964,8 +4240,12 @@
       <c r="H31" s="22">
         <v>208</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>150.50163434299412</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="20">
         <v>30</v>
       </c>
@@ -2987,8 +4267,12 @@
       <c r="H32" s="22">
         <v>202</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>138.0015253867945</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="20">
         <v>31</v>
       </c>
@@ -3010,8 +4294,12 @@
       <c r="H33" s="22">
         <v>195</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>131.5014164305949</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="20">
         <v>32</v>
       </c>
@@ -3033,8 +4321,12 @@
       <c r="H34" s="22">
         <v>189</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>120.50130747439529</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>33</v>
       </c>
@@ -3056,8 +4348,12 @@
       <c r="H35" s="22">
         <v>184</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>114.00130747439528</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="26">
         <v>34</v>
       </c>
@@ -3079,8 +4375,12 @@
       <c r="H36" s="28">
         <v>178</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>105.00119851819568</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="45">
         <v>35</v>
       </c>
@@ -3102,8 +4402,12 @@
       <c r="H37" s="34">
         <v>173</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>194.00217912399214</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>36</v>
       </c>
@@ -3125,8 +4429,12 @@
       <c r="H38" s="30">
         <v>169</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>184.00196121159294</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="20">
         <v>37</v>
       </c>
@@ -3148,8 +4456,12 @@
       <c r="H39" s="22">
         <v>164</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>174.00196121159291</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="20">
         <v>38</v>
       </c>
@@ -3171,8 +4483,12 @@
       <c r="H40" s="22">
         <v>160</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>164.00174329919372</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="20">
         <v>39</v>
       </c>
@@ -3194,8 +4510,12 @@
       <c r="H41" s="22">
         <v>156</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>159.00174329919372</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="20">
         <v>40</v>
       </c>
@@ -3217,8 +4537,12 @@
       <c r="H42" s="22">
         <v>152</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>143.0015253867945</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="20">
         <v>41</v>
       </c>
@@ -3240,8 +4564,12 @@
       <c r="H43" s="22">
         <v>148</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>133.0015253867945</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="20">
         <v>42</v>
       </c>
@@ -3263,8 +4591,12 @@
       <c r="H44" s="22">
         <v>145</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>127.00130747439529</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="20">
         <v>43</v>
       </c>
@@ -3286,8 +4618,12 @@
       <c r="H45" s="22">
         <v>141</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>117.00130747439508</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="20">
         <v>44</v>
       </c>
@@ -3309,8 +4645,12 @@
       <c r="H46" s="22">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>112.00130747439508</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="20">
         <v>45</v>
       </c>
@@ -3332,8 +4672,12 @@
       <c r="H47" s="22">
         <v>135</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>107.00108956199585</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="20">
         <v>46</v>
       </c>
@@ -3355,8 +4699,12 @@
       <c r="H48" s="22">
         <v>132</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>103.00108956199607</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="20">
         <v>47</v>
       </c>
@@ -3378,8 +4726,12 @@
       <c r="H49" s="22">
         <v>129</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>96.001089561995855</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="20">
         <v>48</v>
       </c>
@@ -3401,8 +4753,12 @@
       <c r="H50" s="22">
         <v>127</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>94.001089561996068</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="20">
         <v>49</v>
       </c>
@@ -3424,8 +4780,12 @@
       <c r="H51" s="22">
         <v>124</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>85.00087164959686</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="20">
         <v>50</v>
       </c>
@@ -3447,8 +4807,12 @@
       <c r="H52" s="22">
         <v>122</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>84.00087164959686</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="20">
         <v>51</v>
       </c>
@@ -3470,8 +4834,12 @@
       <c r="H53" s="22">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>82.00087164959686</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="20">
         <v>52</v>
       </c>
@@ -3493,8 +4861,12 @@
       <c r="H54" s="22">
         <v>117</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>80.00087164959686</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="20">
         <v>53</v>
       </c>
@@ -3516,8 +4888,12 @@
       <c r="H55" s="22">
         <v>115</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>75.00087164959686</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="20">
         <v>54</v>
       </c>
@@ -3539,8 +4915,12 @@
       <c r="H56" s="22">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>70.00087164959686</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="20">
         <v>55</v>
       </c>
@@ -3562,8 +4942,12 @@
       <c r="H57" s="22">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>66.000653737197652</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="20">
         <v>56</v>
       </c>
@@ -3585,8 +4969,12 @@
       <c r="H58" s="22">
         <v>109</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>58.000653737197638</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" s="20">
         <v>57</v>
       </c>
@@ -3608,8 +4996,12 @@
       <c r="H59" s="22">
         <v>107</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>58.000653737197638</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" s="20">
         <v>58</v>
       </c>
@@ -3631,8 +5023,12 @@
       <c r="H60" s="22">
         <v>105</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <f t="shared" si="0"/>
+        <v>52.000653737197432</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="20">
         <v>59</v>
       </c>
@@ -3654,8 +5050,12 @@
       <c r="H61" s="22">
         <v>103</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>51.000653737197645</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="20">
         <v>60</v>
       </c>
@@ -3677,8 +5077,12 @@
       <c r="H62" s="22">
         <v>101</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>49.00043582479843</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="20">
         <v>61</v>
       </c>
@@ -3700,8 +5104,12 @@
       <c r="H63" s="22">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <f t="shared" si="0"/>
+        <v>47.000435824798423</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" s="20">
         <v>62</v>
       </c>
@@ -3723,8 +5131,12 @@
       <c r="H64" s="22">
         <v>98</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <f t="shared" si="0"/>
+        <v>46.00043582479843</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" s="20">
         <v>63</v>
       </c>
@@ -3746,8 +5158,12 @@
       <c r="H65" s="22">
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <f t="shared" si="0"/>
+        <v>45.00043582479843</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" s="20">
         <v>64</v>
       </c>
@@ -3769,8 +5185,12 @@
       <c r="H66" s="22">
         <v>95</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <f t="shared" si="0"/>
+        <v>43.00043582479843</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" s="20">
         <v>65</v>
       </c>
@@ -3792,8 +5212,12 @@
       <c r="H67" s="22">
         <v>93</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <f t="shared" si="0"/>
+        <v>40.00043582479843</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" s="20">
         <v>66</v>
       </c>
@@ -3815,8 +5239,12 @@
       <c r="H68" s="22">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <f t="shared" ref="J68:J102" si="1">F68/D68</f>
+        <v>37.00043582479843</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" s="20">
         <v>67</v>
       </c>
@@ -3838,8 +5266,12 @@
       <c r="H69" s="22">
         <v>91</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <f t="shared" si="1"/>
+        <v>37.00043582479843</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" s="20">
         <v>68</v>
       </c>
@@ -3861,8 +5293,12 @@
       <c r="H70" s="22">
         <v>89</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <f t="shared" si="1"/>
+        <v>37.00043582479843</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" s="20">
         <v>69</v>
       </c>
@@ -3884,8 +5320,12 @@
       <c r="H71" s="22">
         <v>88</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <f t="shared" si="1"/>
+        <v>36.00043582479843</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" s="20">
         <v>70</v>
       </c>
@@ -3907,8 +5347,12 @@
       <c r="H72" s="22">
         <v>87</v>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <f t="shared" si="1"/>
+        <v>36.00043582479843</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" s="20">
         <v>71</v>
       </c>
@@ -3930,8 +5374,12 @@
       <c r="H73" s="22">
         <v>85</v>
       </c>
-    </row>
-    <row r="74" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>36.00043582479843</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="26">
         <v>72</v>
       </c>
@@ -3953,8 +5401,12 @@
       <c r="H74" s="28">
         <v>84</v>
       </c>
-    </row>
-    <row r="75" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J74">
+        <f t="shared" si="1"/>
+        <v>36.00043582479843</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="46">
         <v>73</v>
       </c>
@@ -3976,8 +5428,12 @@
       <c r="H75" s="34">
         <v>83</v>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <f t="shared" si="1"/>
+        <v>34.00043582479843</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
         <v>74</v>
       </c>
@@ -3999,8 +5455,12 @@
       <c r="H76" s="30">
         <v>82</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <f t="shared" si="1"/>
+        <v>32.00043582479843</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B77" s="20">
         <v>75</v>
       </c>
@@ -4022,8 +5482,12 @@
       <c r="H77" s="22">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <f t="shared" si="1"/>
+        <v>29.000217912399215</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" s="23">
         <v>76</v>
       </c>
@@ -4045,8 +5509,12 @@
       <c r="H78" s="25">
         <v>80</v>
       </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <f t="shared" si="1"/>
+        <v>26.000217912399215</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" s="20">
         <v>77</v>
       </c>
@@ -4068,8 +5536,12 @@
       <c r="H79" s="22">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <f t="shared" si="1"/>
+        <v>25.000217912399215</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" s="20">
         <v>78</v>
       </c>
@@ -4091,8 +5563,12 @@
       <c r="H80" s="22">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <f t="shared" si="1"/>
+        <v>24.000217912398995</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="20">
         <v>79</v>
       </c>
@@ -4114,8 +5590,12 @@
       <c r="H81" s="22">
         <v>77</v>
       </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <f t="shared" si="1"/>
+        <v>24.000217912398995</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="20">
         <v>80</v>
       </c>
@@ -4137,8 +5617,12 @@
       <c r="H82" s="22">
         <v>76</v>
       </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <f t="shared" si="1"/>
+        <v>24.000217912398995</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="20">
         <v>81</v>
       </c>
@@ -4160,8 +5644,12 @@
       <c r="H83" s="22">
         <v>75</v>
       </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <f t="shared" si="1"/>
+        <v>22.000217912399211</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="20">
         <v>82</v>
       </c>
@@ -4183,8 +5671,12 @@
       <c r="H84" s="22">
         <v>74</v>
       </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <f t="shared" si="1"/>
+        <v>20.000217912399215</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="20">
         <v>83</v>
       </c>
@@ -4206,8 +5698,12 @@
       <c r="H85" s="22">
         <v>73</v>
       </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <f t="shared" si="1"/>
+        <v>20.000217912399215</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="20">
         <v>84</v>
       </c>
@@ -4229,8 +5725,12 @@
       <c r="H86" s="22">
         <v>72</v>
       </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <f t="shared" si="1"/>
+        <v>19.00021791239919</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="20">
         <v>85</v>
       </c>
@@ -4252,8 +5752,12 @@
       <c r="H87" s="22">
         <v>71</v>
       </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>18.000217912399215</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="20">
         <v>86</v>
       </c>
@@ -4275,8 +5779,12 @@
       <c r="H88" s="22">
         <v>70</v>
       </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <f t="shared" si="1"/>
+        <v>17.000217912399215</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="20">
         <v>87</v>
       </c>
@@ -4298,8 +5806,12 @@
       <c r="H89" s="22">
         <v>69</v>
       </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <f t="shared" si="1"/>
+        <v>17.000217912399215</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="20">
         <v>88</v>
       </c>
@@ -4321,8 +5833,12 @@
       <c r="H90" s="22">
         <v>69</v>
       </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <f t="shared" si="1"/>
+        <v>17.000217912399215</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="20">
         <v>89</v>
       </c>
@@ -4344,8 +5860,16 @@
       <c r="H91" s="22">
         <v>68</v>
       </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <f t="shared" si="1"/>
+        <v>16.000217912399215</v>
+      </c>
+      <c r="L91">
+        <f>367/46</f>
+        <v>7.9782608695652177</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="20">
         <v>90</v>
       </c>
@@ -4367,8 +5891,12 @@
       <c r="H92" s="22">
         <v>67</v>
       </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <f t="shared" si="1"/>
+        <v>15.000217912399213</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" s="20">
         <v>91</v>
       </c>
@@ -4390,8 +5918,12 @@
       <c r="H93" s="22">
         <v>66</v>
       </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <f t="shared" si="1"/>
+        <v>14.000217912399215</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" s="20">
         <v>92</v>
       </c>
@@ -4413,8 +5945,12 @@
       <c r="H94" s="22">
         <v>66</v>
       </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J94">
+        <f t="shared" si="1"/>
+        <v>13.000217912399215</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="20">
         <v>93</v>
       </c>
@@ -4436,8 +5972,12 @@
       <c r="H95" s="22">
         <v>65</v>
       </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J95">
+        <f t="shared" si="1"/>
+        <v>13.000217912399215</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" s="20">
         <v>94</v>
       </c>
@@ -4459,8 +5999,12 @@
       <c r="H96" s="22">
         <v>64</v>
       </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J96">
+        <f t="shared" si="1"/>
+        <v>11.000217912399215</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97" s="20">
         <v>95</v>
       </c>
@@ -4482,8 +6026,12 @@
       <c r="H97" s="22">
         <v>63</v>
       </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J97">
+        <f t="shared" si="1"/>
+        <v>11.000217912399215</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="20">
         <v>96</v>
       </c>
@@ -4505,8 +6053,12 @@
       <c r="H98" s="22">
         <v>63</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J98">
+        <f t="shared" si="1"/>
+        <v>10.000217912399215</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B99" s="26">
         <v>97</v>
       </c>
@@ -4528,8 +6080,12 @@
       <c r="H99" s="28">
         <v>62</v>
       </c>
-    </row>
-    <row r="100" spans="2:8" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J99">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999982</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="45">
         <v>98</v>
       </c>
@@ -4551,8 +6107,12 @@
       <c r="H100" s="34">
         <v>61</v>
       </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J100">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
         <v>99</v>
       </c>
@@ -4574,8 +6134,12 @@
       <c r="H101" s="30">
         <v>61</v>
       </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102" s="20">
         <v>100</v>
       </c>
@@ -4596,11 +6160,16 @@
       </c>
       <c r="H102" s="22">
         <v>60</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4608,8 +6177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -4659,7 +6228,7 @@
       <c r="B4" s="49">
         <v>10</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="71">
         <v>0.123904</v>
       </c>
       <c r="D4" s="63">
@@ -4710,7 +6279,7 @@
       <c r="B7" s="50">
         <v>35</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="73">
         <v>4.5890000000000002E-3</v>
       </c>
       <c r="D7" s="63">
@@ -4798,7 +6367,7 @@
       <c r="C12" s="54">
         <v>4.5890000000000002E-3</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="72">
         <v>0.13308200000000001</v>
       </c>
       <c r="E12" s="58">
@@ -4849,7 +6418,7 @@
       <c r="C15" s="54">
         <v>4.5890000000000002E-3</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="74">
         <v>3.6712000000000002E-2</v>
       </c>
       <c r="E15" s="58">

</xml_diff>